<commit_message>
Created new Empty Project Raumplanung Core
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_JanMair_739694.xlsx
+++ b/Additional Files/Zeiterfassung_JanMair_739694.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>2h</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Zeiterfassungsdokument erstellt, Vision verfasst</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>Einarbeitung/Tutorials anschauen bezüglich asp.net core</t>
   </si>
 </sst>
 </file>
@@ -378,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,6 +428,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>42722</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Implemented a good chunk of the AuthentificationLogic
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_JanMair_739694.xlsx
+++ b/Additional Files/Zeiterfassung_JanMair_739694.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>2h</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Einarbeitung/Tutorials anschauen bezüglich asp.net core</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Mit Code experimentiert, neues Leeres Projekt erstellt, Designskizze angefangen</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,6 +445,17 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>42723</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
weiter übersetzt, zeiterfassung updatet
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_JanMair_739694.xlsx
+++ b/Additional Files/Zeiterfassung_JanMair_739694.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Datum</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>adminseite und adminseitencontroller erstellt mit admin authentifizierung, funktionierenden mailsender eingebaut, passwordrücksetzung mit mail eingebaut, emailbestätigung eingebaut, anrede,vorname,nachname hinzugefügt,erste seite ist unterschiedlich abhängig davon ob man eingeloggt ist oder nicht, manche sachen übersetzt(noch nicht alles), fehler bei registrierung behoben</t>
+  </si>
+  <si>
+    <t>zuende übersetzt von allem was zu dem zeitpunkt existiert hat und benötigt wird/werden wird</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,6 +503,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42728</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
tauschen mit allem außer datenbanksachen, tauschanfragenseite als prototyp zeiterfassung aktualisiert
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_JanMair_739694.xlsx
+++ b/Additional Files/Zeiterfassung_JanMair_739694.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Datum</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>zuende übersetzt von allem was zu dem zeitpunkt existiert hat und benötigt wird/werden wird</t>
+  </si>
+  <si>
+    <t>accountmanage seit mit passwort ändern,reservierungen löschbar, details,tauschseite und anfragenseite(noch ohne datenbankanbindung)</t>
   </si>
 </sst>
 </file>
@@ -85,10 +88,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -393,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +429,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>42719</v>
       </c>
       <c r="B3">
@@ -512,6 +514,17 @@
       </c>
       <c r="C10" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42731</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
alles von anfragen geht auf view seite, datenbankimplementierung fehlt
</commit_message>
<xml_diff>
--- a/Additional Files/Zeiterfassung_JanMair_739694.xlsx
+++ b/Additional Files/Zeiterfassung_JanMair_739694.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Datum</t>
   </si>
@@ -52,7 +52,10 @@
     <t>zuende übersetzt von allem was zu dem zeitpunkt existiert hat und benötigt wird/werden wird</t>
   </si>
   <si>
-    <t>accountmanage seit mit passwort ändern,reservierungen löschbar, details,tauschseite und anfragenseite(noch ohne datenbankanbindung)</t>
+    <t>anfragenseite komplettes layout und controllerfunktionen,detailseite gefüllt</t>
+  </si>
+  <si>
+    <t>accountmanage seit mit passwort ändern,reservierungen löschbar, details,tauschseite</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +527,17 @@
         <v>6</v>
       </c>
       <c r="C11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>42732</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>